<commit_message>
Updating risk assessment, diagrams
</commit_message>
<xml_diff>
--- a/documentation/risk-assessment.xlsx
+++ b/documentation/risk-assessment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44749\Desktop\QA\Projects\IMS-22JulyEnable3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44749\Desktop\QA\Projects\IMS-22JulyEnable3\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9481812E-FD6A-4942-9135-43CE4193CD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735647BC-B082-45A5-B5B9-D5C74A9CD2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
   <si>
     <t>Risk Matrices</t>
   </si>
@@ -111,16 +111,64 @@
     <t>Risk Level</t>
   </si>
   <si>
-    <t>RSI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">My wrists could be aching </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ensure I move wrists about </t>
-  </si>
-  <si>
-    <t>To keep my wrists safe for the future</t>
+    <t>Faults in my computer or system</t>
+  </si>
+  <si>
+    <t>A fault in my computer or a complete break could possibly happen, and would lead to loss of the local repository and an inability to carry on the project.</t>
+  </si>
+  <si>
+    <t>I back up my computer regularly and also push to Git regularly so that if something were to happen I would always be able to access a recent version.</t>
+  </si>
+  <si>
+    <t>To make sure my data and dev environment is secure in case of an  accident.</t>
+  </si>
+  <si>
+    <t>Loss of internet during the project</t>
+  </si>
+  <si>
+    <t>Losing signal for the internet is a possibility, and has happened previously during my time at QA. Would lead to inability to push to Git/to access online repository.</t>
+  </si>
+  <si>
+    <t>Always keep a local repository so code is accessible even if online.</t>
+  </si>
+  <si>
+    <t>To ensure that time is not wasted on internet issues and to keep both online and local repositorys.</t>
+  </si>
+  <si>
+    <t>Corrupted file</t>
+  </si>
+  <si>
+    <t>The file which stores all the documents and code for the project has a possibility to become corrupted due to many unavoidable reasons.</t>
+  </si>
+  <si>
+    <t>To minimise the risks of data corruption by backing up often.</t>
+  </si>
+  <si>
+    <t>Bugs/unthrown exceptions in the code</t>
+  </si>
+  <si>
+    <t>Project not being ready by the deadline</t>
+  </si>
+  <si>
+    <t>Bugs and unthrown exceptions could make it to the final submission version of the project.</t>
+  </si>
+  <si>
+    <t>Thorough testing aiming for as much coverage as possible, as well as using the project often to ensure that it is performing SQL database operations correctly.</t>
+  </si>
+  <si>
+    <t>To be able to have functional and high quality code in the final version. Risk depends on the severity of the bug.</t>
+  </si>
+  <si>
+    <t>Backing up to Github, including backing up the schema so that the database is not lost either. If the database were corrupted for a working version of this application it would be much higher impact.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To ensure that I use my time as effectively as possible to avoid missing the deadline. </t>
+  </si>
+  <si>
+    <t>To ensure that I plan my sprints appropriately so that my time is used as effectively as possible to avoid missing the deadline. Also, work first on a MVP before adding extra features.</t>
+  </si>
+  <si>
+    <t>If the project is not complete by the deadline, it could miss testing or not be fully functional.</t>
   </si>
 </sst>
 </file>
@@ -142,7 +190,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +227,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -192,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -200,12 +254,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,15 +580,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H17"/>
+  <dimension ref="B1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" customWidth="1"/>
     <col min="3" max="3" width="35.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.453125" customWidth="1"/>
     <col min="5" max="5" width="31.81640625" customWidth="1"/>
@@ -563,19 +623,19 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -583,19 +643,19 @@
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -603,19 +663,19 @@
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -623,19 +683,19 @@
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -643,19 +703,19 @@
       <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -682,51 +742,118 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="30" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
+    <row r="12" spans="2:8" ht="73" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="2" t="s">
+      <c r="F12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="2:8" ht="105.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="2:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="4:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="2:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="2:8" ht="85" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="2:8" ht="91.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="3:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="2"/>
       <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="3:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -734,26 +861,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d63dcd26-5253-4c87-aabc-8b4306a65eaf">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="43f262de-373e-47a6-9b14-73d0f614ebcb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085A4A6BC947BC6458D5FA78AC51178F5" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c2300d6ce10fd547c5cdddf99baa3a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d63dcd26-5253-4c87-aabc-8b4306a65eaf" xmlns:ns3="43f262de-373e-47a6-9b14-73d0f614ebcb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="312c6d9a31e5bb64cb8da0cd8a13f183" ns2:_="" ns3:_="">
     <xsd:import namespace="d63dcd26-5253-4c87-aabc-8b4306a65eaf"/>
@@ -970,26 +1077,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA03BEC0-4179-4E6D-8A2C-E738731D0931}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d63dcd26-5253-4c87-aabc-8b4306a65eaf"/>
-    <ds:schemaRef ds:uri="43f262de-373e-47a6-9b14-73d0f614ebcb"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0A4A8A4-0C2B-4B8F-AD2C-30B3C4CC8D49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d63dcd26-5253-4c87-aabc-8b4306a65eaf">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="43f262de-373e-47a6-9b14-73d0f614ebcb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD478693-D84F-44E7-BC89-A0B000CE687F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1006,4 +1114,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0A4A8A4-0C2B-4B8F-AD2C-30B3C4CC8D49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA03BEC0-4179-4E6D-8A2C-E738731D0931}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d63dcd26-5253-4c87-aabc-8b4306a65eaf"/>
+    <ds:schemaRef ds:uri="43f262de-373e-47a6-9b14-73d0f614ebcb"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>